<commit_message>
data spec updated with review data
</commit_message>
<xml_diff>
--- a/hotel_data_spec.xlsx
+++ b/hotel_data_spec.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karen\Desktop\eskwelabs\dsf10_capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{615EF6A6-1C8E-47BF-BE18-282D3747D95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B7AD59F-8196-412A-8C02-8BCD89FA90DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{7C338DF9-90F4-479C-8007-393E05CBEC2B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24420" windowHeight="16220" xr2:uid="{7C338DF9-90F4-479C-8007-393E05CBEC2B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="hotel_info" sheetId="1" r:id="rId1"/>
+    <sheet name="hotel_reviews" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>column name</t>
   </si>
@@ -41,12 +42,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>hotel_name</t>
-  </si>
-  <si>
-    <t>star</t>
-  </si>
-  <si>
     <t>star rating (1-5)</t>
   </si>
   <si>
@@ -54,9 +49,6 @@
   </si>
   <si>
     <t>adress of the property</t>
-  </si>
-  <si>
-    <t>location_score</t>
   </si>
   <si>
     <t>review_rating</t>
@@ -197,27 +189,9 @@
     <t>url of hotel in booking.com</t>
   </si>
   <si>
-    <t>hotel_name_from_all_urls</t>
-  </si>
-  <si>
     <t>name of hotel</t>
   </si>
   <si>
-    <t>location_from_all_urls</t>
-  </si>
-  <si>
-    <t>city level location</t>
-  </si>
-  <si>
-    <t>distance_from_center</t>
-  </si>
-  <si>
-    <t>distance (in km) of the hotel from the center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">based on review-score-badge element </t>
-  </si>
-  <si>
     <t>overall score from guest reviews</t>
   </si>
   <si>
@@ -225,12 +199,6 @@
   </si>
   <si>
     <t>others</t>
-  </si>
-  <si>
-    <t>this score is based on guest reviews, this is the highest rating of a specific category not necessarily the location only</t>
-  </si>
-  <si>
-    <t>we can drop this since this information can be found in sub_ratings</t>
   </si>
   <si>
     <t>elements inside list is duplicated, clean to only include unique values</t>
@@ -253,12 +221,132 @@
       <t xml:space="preserve"> 1 row = 1 property (hotel)</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table name: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hotel_info_final</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Granularity:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 row = 1 review per property</t>
+    </r>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>room_type</t>
+  </si>
+  <si>
+    <t>nights_stayed</t>
+  </si>
+  <si>
+    <t>month_stayed</t>
+  </si>
+  <si>
+    <t>occupant_type</t>
+  </si>
+  <si>
+    <t>from_country</t>
+  </si>
+  <si>
+    <t>review_score</t>
+  </si>
+  <si>
+    <t>date_reviewed</t>
+  </si>
+  <si>
+    <t>short_review</t>
+  </si>
+  <si>
+    <t>positive_review</t>
+  </si>
+  <si>
+    <t>negative_review</t>
+  </si>
+  <si>
+    <t>Columns need to be transformed to correct format (currently all are objects)</t>
+  </si>
+  <si>
+    <t>name of reviewer</t>
+  </si>
+  <si>
+    <t>can be anonymous</t>
+  </si>
+  <si>
+    <t>room type similar to hotel_info</t>
+  </si>
+  <si>
+    <t>number of nights stayed</t>
+  </si>
+  <si>
+    <t>keep only numbers</t>
+  </si>
+  <si>
+    <t>month-year the traveler stayed</t>
+  </si>
+  <si>
+    <t>values: couple, family, solo traveler</t>
+  </si>
+  <si>
+    <t>country of origin</t>
+  </si>
+  <si>
+    <t>overall review score</t>
+  </si>
+  <si>
+    <t>month-year of review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overall review </t>
+  </si>
+  <si>
+    <t>positive review</t>
+  </si>
+  <si>
+    <t>negative review</t>
+  </si>
+  <si>
+    <t>link to hotel page</t>
+  </si>
+  <si>
+    <t>hotel_name_</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>room_price_dict</t>
+  </si>
+  <si>
+    <t>room type and price dictionary, cheapest price per room type</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +358,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -295,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -312,6 +408,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB8882FD-1302-4854-9A4B-F0BF2D5FFB4E}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -644,145 +747,164 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>59</v>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -790,13 +912,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -804,148 +926,248 @@
         <v>30</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CA04A6-1931-4597-B4B7-33F07AF27C61}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>55</v>
+      <c r="C17" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>